<commit_message>
CSRs tests working on 32b and 64b variants
Signed-off-by: Anderson Ignacio <anderson@aignacio.com>
</commit_message>
<xml_diff>
--- a/csr_dma.xlsx
+++ b/csr_dma.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10111"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A411B6D7-A05B-6E4B-8406-BA089ABEF5FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8F5680D-00B8-F141-A0EF-6B5C93AA68F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7740" yWindow="14360" windowWidth="49080" windowHeight="24140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="820" yWindow="17440" windowWidth="49080" windowHeight="24140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="block_0" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="66">
   <si>
     <t>block name</t>
     <phoneticPr fontId="1"/>
@@ -199,6 +199,42 @@
   </si>
   <si>
     <t>Error type - Operation / Configuration</t>
+  </si>
+  <si>
+    <t>0x10</t>
+  </si>
+  <si>
+    <t>0x00</t>
+  </si>
+  <si>
+    <t>0x08</t>
+  </si>
+  <si>
+    <t>in the assignment = width:lsb:sequence_size:step</t>
+  </si>
+  <si>
+    <t>0x20</t>
+  </si>
+  <si>
+    <t>32:0</t>
+  </si>
+  <si>
+    <t>1:64</t>
+  </si>
+  <si>
+    <t>32:64</t>
+  </si>
+  <si>
+    <t>32:128</t>
+  </si>
+  <si>
+    <t>1:192</t>
+  </si>
+  <si>
+    <t>32</t>
+  </si>
+  <si>
+    <t>We need to align each register to 64b to support the two designs 32/64b AXI_DATA_WIDTH</t>
   </si>
 </sst>
 </file>
@@ -360,7 +396,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -400,6 +436,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -709,15 +748,16 @@
   <dimension ref="B1:K69"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="210" zoomScaleNormal="210" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="13.1640625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.1640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9" style="1"/>
     <col min="9" max="9" width="11.33203125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="20.33203125" style="1" bestFit="1" customWidth="1"/>
@@ -731,6 +771,9 @@
       <c r="C1" s="2" t="s">
         <v>12</v>
       </c>
+      <c r="E1" s="1" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="2" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B2" s="1" t="s">
@@ -738,6 +781,9 @@
       </c>
       <c r="C2" s="2">
         <v>256</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="3" spans="2:11" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
@@ -774,12 +820,14 @@
       </c>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B5" s="19" t="s">
+      <c r="B5" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="16"/>
-      <c r="D5" s="16"/>
-      <c r="E5" s="19"/>
+      <c r="C5" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="D5" s="17"/>
+      <c r="E5" s="20"/>
       <c r="F5" s="3" t="s">
         <v>19</v>
       </c>
@@ -798,10 +846,10 @@
       </c>
     </row>
     <row r="6" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B6" s="20"/>
-      <c r="C6" s="18"/>
-      <c r="D6" s="18"/>
-      <c r="E6" s="20"/>
+      <c r="B6" s="21"/>
+      <c r="C6" s="19"/>
+      <c r="D6" s="19"/>
+      <c r="E6" s="21"/>
       <c r="F6" s="3" t="s">
         <v>20</v>
       </c>
@@ -820,12 +868,14 @@
       </c>
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B7" s="21" t="s">
+      <c r="B7" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="22"/>
-      <c r="D7" s="22"/>
-      <c r="E7" s="21"/>
+      <c r="C7" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="D7" s="23"/>
+      <c r="E7" s="22"/>
       <c r="F7" s="13" t="s">
         <v>22</v>
       </c>
@@ -844,10 +894,10 @@
       </c>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B8" s="21"/>
-      <c r="C8" s="22"/>
-      <c r="D8" s="22"/>
-      <c r="E8" s="21"/>
+      <c r="B8" s="22"/>
+      <c r="C8" s="23"/>
+      <c r="D8" s="23"/>
+      <c r="E8" s="22"/>
       <c r="F8" s="13" t="s">
         <v>21</v>
       </c>
@@ -866,10 +916,10 @@
       </c>
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B9" s="21"/>
-      <c r="C9" s="22"/>
-      <c r="D9" s="22"/>
-      <c r="E9" s="21"/>
+      <c r="B9" s="22"/>
+      <c r="C9" s="23"/>
+      <c r="D9" s="23"/>
+      <c r="E9" s="22"/>
       <c r="F9" s="13" t="s">
         <v>49</v>
       </c>
@@ -882,7 +932,7 @@
       <c r="I9" s="14">
         <v>0</v>
       </c>
-      <c r="J9" s="15" t="s">
+      <c r="J9" s="16" t="s">
         <v>51</v>
       </c>
       <c r="K9" s="4" t="s">
@@ -890,17 +940,19 @@
       </c>
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B10" s="16" t="s">
+      <c r="B10" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="C10" s="16"/>
-      <c r="D10" s="16"/>
-      <c r="E10" s="16"/>
+      <c r="C10" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="D10" s="17"/>
+      <c r="E10" s="17"/>
       <c r="F10" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="G10" s="14">
-        <v>32</v>
+      <c r="G10" s="15" t="s">
+        <v>64</v>
       </c>
       <c r="H10" s="14" t="s">
         <v>18</v>
@@ -914,15 +966,15 @@
       </c>
     </row>
     <row r="11" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B11" s="17"/>
-      <c r="C11" s="17"/>
-      <c r="D11" s="17"/>
-      <c r="E11" s="17"/>
+      <c r="B11" s="18"/>
+      <c r="C11" s="18"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="18"/>
       <c r="F11" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="G11" s="14">
-        <v>1</v>
+      <c r="G11" s="15" t="s">
+        <v>60</v>
       </c>
       <c r="H11" s="14" t="s">
         <v>18</v>
@@ -936,14 +988,14 @@
       </c>
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B12" s="17"/>
-      <c r="C12" s="17"/>
-      <c r="D12" s="17"/>
-      <c r="E12" s="17"/>
+      <c r="B12" s="18"/>
+      <c r="C12" s="18"/>
+      <c r="D12" s="18"/>
+      <c r="E12" s="18"/>
       <c r="F12" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="G12" s="14">
+      <c r="G12" s="15">
         <v>1</v>
       </c>
       <c r="H12" s="14" t="s">
@@ -958,14 +1010,14 @@
       </c>
     </row>
     <row r="13" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B13" s="17"/>
-      <c r="C13" s="17"/>
-      <c r="D13" s="17"/>
-      <c r="E13" s="17"/>
+      <c r="B13" s="18"/>
+      <c r="C13" s="18"/>
+      <c r="D13" s="18"/>
+      <c r="E13" s="18"/>
       <c r="F13" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="G13" s="14">
+      <c r="G13" s="15">
         <v>1</v>
       </c>
       <c r="H13" s="14" t="s">
@@ -980,19 +1032,21 @@
       </c>
     </row>
     <row r="14" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B14" s="16" t="s">
+      <c r="B14" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="C14" s="16"/>
-      <c r="D14" s="16" t="s">
+      <c r="C14" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="D14" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="E14" s="16"/>
+      <c r="E14" s="17"/>
       <c r="F14" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="G14" s="14">
-        <v>32</v>
+      <c r="G14" s="15" t="s">
+        <v>59</v>
       </c>
       <c r="H14" s="14" t="s">
         <v>39</v>
@@ -1006,15 +1060,15 @@
       </c>
     </row>
     <row r="15" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B15" s="17"/>
-      <c r="C15" s="17"/>
-      <c r="D15" s="17"/>
-      <c r="E15" s="17"/>
+      <c r="B15" s="18"/>
+      <c r="C15" s="18"/>
+      <c r="D15" s="18"/>
+      <c r="E15" s="18"/>
       <c r="F15" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="G15" s="14">
-        <v>32</v>
+      <c r="G15" s="15" t="s">
+        <v>61</v>
       </c>
       <c r="H15" s="14" t="s">
         <v>39</v>
@@ -1028,15 +1082,15 @@
       </c>
     </row>
     <row r="16" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B16" s="17"/>
-      <c r="C16" s="17"/>
-      <c r="D16" s="17"/>
-      <c r="E16" s="17"/>
+      <c r="B16" s="18"/>
+      <c r="C16" s="18"/>
+      <c r="D16" s="18"/>
+      <c r="E16" s="18"/>
       <c r="F16" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="G16" s="14">
-        <v>32</v>
+      <c r="G16" s="15" t="s">
+        <v>62</v>
       </c>
       <c r="H16" s="14" t="s">
         <v>39</v>
@@ -1050,15 +1104,15 @@
       </c>
     </row>
     <row r="17" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B17" s="17"/>
-      <c r="C17" s="17"/>
-      <c r="D17" s="17"/>
-      <c r="E17" s="17"/>
+      <c r="B17" s="18"/>
+      <c r="C17" s="18"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="18"/>
       <c r="F17" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="G17" s="14">
-        <v>1</v>
+      <c r="G17" s="15" t="s">
+        <v>63</v>
       </c>
       <c r="H17" s="14" t="s">
         <v>39</v>
@@ -1072,14 +1126,14 @@
       </c>
     </row>
     <row r="18" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B18" s="17"/>
-      <c r="C18" s="17"/>
-      <c r="D18" s="17"/>
-      <c r="E18" s="17"/>
+      <c r="B18" s="18"/>
+      <c r="C18" s="18"/>
+      <c r="D18" s="18"/>
+      <c r="E18" s="18"/>
       <c r="F18" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="G18" s="13" t="s">
+      <c r="G18" s="15" t="s">
         <v>11</v>
       </c>
       <c r="H18" s="14" t="s">
@@ -1094,15 +1148,15 @@
       </c>
     </row>
     <row r="19" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B19" s="18"/>
-      <c r="C19" s="18"/>
-      <c r="D19" s="18"/>
-      <c r="E19" s="18"/>
+      <c r="B19" s="19"/>
+      <c r="C19" s="19"/>
+      <c r="D19" s="19"/>
+      <c r="E19" s="19"/>
       <c r="F19" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="G19" s="14">
-        <v>1</v>
+      <c r="G19" s="15" t="s">
+        <v>11</v>
       </c>
       <c r="H19" s="14" t="s">
         <v>39</v>
@@ -1279,7 +1333,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="G18 G8:G9 G5:G7" numberStoredAsText="1"/>
+    <ignoredError sqref="G18:G19 G8:G10 G5:G7" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added DMA FSM and func wrapper
Signed-off-by: Anderson Ignacio <anderson@aignacio.com>
</commit_message>
<xml_diff>
--- a/csr_dma.xlsx
+++ b/csr_dma.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10520"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8F5680D-00B8-F141-A0EF-6B5C93AA68F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E86F390D-0DCA-174B-9D06-3EE740FE81D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="820" yWindow="17440" windowWidth="49080" windowHeight="24140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7660" yWindow="3500" windowWidth="49080" windowHeight="24140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="block_0" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="69">
   <si>
     <t>block name</t>
     <phoneticPr fontId="1"/>
@@ -210,9 +210,6 @@
     <t>0x08</t>
   </si>
   <si>
-    <t>in the assignment = width:lsb:sequence_size:step</t>
-  </si>
-  <si>
     <t>0x20</t>
   </si>
   <si>
@@ -235,13 +232,25 @@
   </si>
   <si>
     <t>We need to align each register to 64b to support the two designs 32/64b AXI_DATA_WIDTH</t>
+  </si>
+  <si>
+    <t>max_burst</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>Max burst length (ALEN) in the AXI txn</t>
+  </si>
+  <si>
+    <t>&gt; assignment = width:lsb:sequence_size:step</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -256,13 +265,39 @@
       <charset val="128"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="10">
@@ -396,74 +431,83 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -745,10 +789,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:K69"/>
+  <dimension ref="B1:K70"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="210" zoomScaleNormal="210" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -772,7 +816,7 @@
         <v>12</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="2" spans="2:11" x14ac:dyDescent="0.2">
@@ -783,399 +827,413 @@
         <v>256</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>57</v>
+        <v>68</v>
       </c>
     </row>
     <row r="3" spans="2:11" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="8" t="s">
+      <c r="E4" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="8" t="s">
+      <c r="F4" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="8" t="s">
+      <c r="G4" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="H4" s="8" t="s">
+      <c r="H4" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="I4" s="7" t="s">
+      <c r="I4" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="J4" s="9" t="s">
+      <c r="J4" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="K4" s="10" t="s">
+      <c r="K4" s="26" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B5" s="20" t="s">
+      <c r="B5" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="17" t="s">
+      <c r="C5" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="D5" s="17"/>
-      <c r="E5" s="20"/>
-      <c r="F5" s="3" t="s">
+      <c r="D5" s="4"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="G5" s="5" t="s">
+      <c r="G5" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="H5" s="3" t="s">
+      <c r="H5" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="I5" s="4">
-        <v>0</v>
-      </c>
-      <c r="J5" s="3"/>
-      <c r="K5" s="4" t="s">
+      <c r="I5" s="7">
+        <v>0</v>
+      </c>
+      <c r="J5" s="5"/>
+      <c r="K5" s="7" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="6" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B6" s="21"/>
-      <c r="C6" s="19"/>
-      <c r="D6" s="19"/>
-      <c r="E6" s="21"/>
-      <c r="F6" s="3" t="s">
+      <c r="B6" s="8"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="G6" s="5" t="s">
+      <c r="G6" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="H6" s="3" t="s">
+      <c r="H6" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="I6" s="4">
-        <v>0</v>
-      </c>
-      <c r="J6" s="3"/>
-      <c r="K6" s="4" t="s">
+      <c r="I6" s="7">
+        <v>0</v>
+      </c>
+      <c r="J6" s="5"/>
+      <c r="K6" s="7" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B7" s="22" t="s">
+      <c r="B7" s="10"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="I7" s="7">
+        <v>255</v>
+      </c>
+      <c r="J7" s="5"/>
+      <c r="K7" s="7" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="8" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B8" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="23" t="s">
+      <c r="C8" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="D7" s="23"/>
-      <c r="E7" s="22"/>
-      <c r="F7" s="13" t="s">
+      <c r="D8" s="14"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="G7" s="14" t="s">
+      <c r="G8" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="H7" s="13" t="s">
+      <c r="H8" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="I7" s="14" t="s">
+      <c r="I8" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="J7" s="13"/>
-      <c r="K7" s="4" t="s">
+      <c r="J8" s="15"/>
+      <c r="K8" s="17" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B8" s="22"/>
-      <c r="C8" s="23"/>
-      <c r="D8" s="23"/>
-      <c r="E8" s="22"/>
-      <c r="F8" s="13" t="s">
+    <row r="9" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B9" s="13"/>
+      <c r="C9" s="14"/>
+      <c r="D9" s="14"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="G8" s="14" t="s">
+      <c r="G9" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="H8" s="13" t="s">
+      <c r="H9" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="I8" s="14">
-        <v>0</v>
-      </c>
-      <c r="J8" s="13"/>
-      <c r="K8" s="4" t="s">
+      <c r="I9" s="16">
+        <v>0</v>
+      </c>
+      <c r="J9" s="15"/>
+      <c r="K9" s="17" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B9" s="22"/>
-      <c r="C9" s="23"/>
-      <c r="D9" s="23"/>
-      <c r="E9" s="22"/>
-      <c r="F9" s="13" t="s">
+    <row r="10" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B10" s="13"/>
+      <c r="C10" s="14"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="G9" s="14" t="s">
+      <c r="G10" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="H9" s="13" t="s">
+      <c r="H10" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="I9" s="14">
-        <v>0</v>
-      </c>
-      <c r="J9" s="16" t="s">
+      <c r="I10" s="16">
+        <v>0</v>
+      </c>
+      <c r="J10" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="K9" s="4" t="s">
+      <c r="K10" s="17" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B10" s="17" t="s">
+    <row r="11" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B11" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="C10" s="17" t="s">
+      <c r="C11" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="D10" s="17"/>
-      <c r="E10" s="17"/>
-      <c r="F10" s="11" t="s">
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="G10" s="15" t="s">
-        <v>64</v>
-      </c>
-      <c r="H10" s="14" t="s">
+      <c r="G11" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="H11" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="I10" s="14">
-        <v>0</v>
-      </c>
-      <c r="J10" s="14"/>
-      <c r="K10" s="14" t="s">
+      <c r="I11" s="6">
+        <v>0</v>
+      </c>
+      <c r="J11" s="6"/>
+      <c r="K11" s="6" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B11" s="18"/>
-      <c r="C11" s="18"/>
-      <c r="D11" s="18"/>
-      <c r="E11" s="18"/>
-      <c r="F11" s="13" t="s">
+    <row r="12" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B12" s="9"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="G11" s="15" t="s">
+      <c r="G12" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="H12" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="I12" s="6">
+        <v>0</v>
+      </c>
+      <c r="J12" s="6"/>
+      <c r="K12" s="6" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="13" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B13" s="9"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="G13" s="12">
+        <v>1</v>
+      </c>
+      <c r="H13" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="I13" s="6">
+        <v>0</v>
+      </c>
+      <c r="J13" s="6"/>
+      <c r="K13" s="6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="14" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B14" s="9"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="G14" s="12">
+        <v>1</v>
+      </c>
+      <c r="H14" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="I14" s="6">
+        <v>0</v>
+      </c>
+      <c r="J14" s="6"/>
+      <c r="K14" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="15" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B15" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="C15" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="D15" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="E15" s="19"/>
+      <c r="F15" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="G15" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="H15" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="I15" s="16">
+        <v>0</v>
+      </c>
+      <c r="J15" s="16"/>
+      <c r="K15" s="16" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="16" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B16" s="20"/>
+      <c r="C16" s="20"/>
+      <c r="D16" s="20"/>
+      <c r="E16" s="20"/>
+      <c r="F16" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="G16" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="H11" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="I11" s="14">
-        <v>0</v>
-      </c>
-      <c r="J11" s="14"/>
-      <c r="K11" s="14" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B12" s="18"/>
-      <c r="C12" s="18"/>
-      <c r="D12" s="18"/>
-      <c r="E12" s="18"/>
-      <c r="F12" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="G12" s="15">
-        <v>1</v>
-      </c>
-      <c r="H12" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="I12" s="14">
-        <v>0</v>
-      </c>
-      <c r="J12" s="14"/>
-      <c r="K12" s="14" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B13" s="18"/>
-      <c r="C13" s="18"/>
-      <c r="D13" s="18"/>
-      <c r="E13" s="18"/>
-      <c r="F13" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="G13" s="15">
-        <v>1</v>
-      </c>
-      <c r="H13" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="I13" s="14">
-        <v>0</v>
-      </c>
-      <c r="J13" s="14"/>
-      <c r="K13" s="14" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B14" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="C14" s="17" t="s">
-        <v>58</v>
-      </c>
-      <c r="D14" s="17" t="s">
-        <v>40</v>
-      </c>
-      <c r="E14" s="17"/>
-      <c r="F14" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="G14" s="15" t="s">
-        <v>59</v>
-      </c>
-      <c r="H14" s="14" t="s">
+      <c r="H16" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="I14" s="14">
-        <v>0</v>
-      </c>
-      <c r="J14" s="14"/>
-      <c r="K14" s="14" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B15" s="18"/>
-      <c r="C15" s="18"/>
-      <c r="D15" s="18"/>
-      <c r="E15" s="18"/>
-      <c r="F15" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="G15" s="15" t="s">
+      <c r="I16" s="16">
+        <v>0</v>
+      </c>
+      <c r="J16" s="16"/>
+      <c r="K16" s="16" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B17" s="20"/>
+      <c r="C17" s="20"/>
+      <c r="D17" s="20"/>
+      <c r="E17" s="20"/>
+      <c r="F17" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="G17" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="H15" s="14" t="s">
+      <c r="H17" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="I15" s="14">
-        <v>0</v>
-      </c>
-      <c r="J15" s="14"/>
-      <c r="K15" s="14" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B16" s="18"/>
-      <c r="C16" s="18"/>
-      <c r="D16" s="18"/>
-      <c r="E16" s="18"/>
-      <c r="F16" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="G16" s="15" t="s">
+      <c r="I17" s="16">
+        <v>0</v>
+      </c>
+      <c r="J17" s="16"/>
+      <c r="K17" s="16" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="18" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B18" s="20"/>
+      <c r="C18" s="20"/>
+      <c r="D18" s="20"/>
+      <c r="E18" s="20"/>
+      <c r="F18" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="G18" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="H16" s="14" t="s">
+      <c r="H18" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="I16" s="14">
-        <v>0</v>
-      </c>
-      <c r="J16" s="14"/>
-      <c r="K16" s="14" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B17" s="18"/>
-      <c r="C17" s="18"/>
-      <c r="D17" s="18"/>
-      <c r="E17" s="18"/>
-      <c r="F17" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="G17" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="H17" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="I17" s="14">
-        <v>0</v>
-      </c>
-      <c r="J17" s="14"/>
-      <c r="K17" s="14" t="s">
+      <c r="I18" s="16">
+        <v>0</v>
+      </c>
+      <c r="J18" s="16"/>
+      <c r="K18" s="16" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B18" s="18"/>
-      <c r="C18" s="18"/>
-      <c r="D18" s="18"/>
-      <c r="E18" s="18"/>
-      <c r="F18" s="13" t="s">
+    <row r="19" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B19" s="20"/>
+      <c r="C19" s="20"/>
+      <c r="D19" s="20"/>
+      <c r="E19" s="20"/>
+      <c r="F19" s="15" t="s">
         <v>33</v>
-      </c>
-      <c r="G18" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="H18" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="I18" s="14">
-        <v>0</v>
-      </c>
-      <c r="J18" s="14"/>
-      <c r="K18" s="14" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B19" s="19"/>
-      <c r="C19" s="19"/>
-      <c r="D19" s="19"/>
-      <c r="E19" s="19"/>
-      <c r="F19" s="13" t="s">
-        <v>41</v>
       </c>
       <c r="G19" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="H19" s="14" t="s">
+      <c r="H19" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="I19" s="14">
-        <v>0</v>
-      </c>
-      <c r="J19" s="14"/>
-      <c r="K19" s="12" t="s">
+      <c r="I19" s="16">
+        <v>0</v>
+      </c>
+      <c r="J19" s="16"/>
+      <c r="K19" s="16" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="20" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B20" s="21"/>
+      <c r="C20" s="21"/>
+      <c r="D20" s="21"/>
+      <c r="E20" s="21"/>
+      <c r="F20" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="G20" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="H20" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="I20" s="16">
+        <v>0</v>
+      </c>
+      <c r="J20" s="16"/>
+      <c r="K20" s="16" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="20" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B20"/>
-      <c r="E20"/>
-      <c r="F20"/>
-      <c r="G20"/>
-      <c r="H20"/>
-      <c r="J20"/>
     </row>
     <row r="21" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B21"/>
@@ -1310,30 +1368,31 @@
     <row r="67" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="68" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="69" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="70" customFormat="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="B14:B19"/>
-    <mergeCell ref="C14:C19"/>
-    <mergeCell ref="D14:D19"/>
-    <mergeCell ref="E14:E19"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="C10:C13"/>
-    <mergeCell ref="B10:B13"/>
-    <mergeCell ref="E10:E13"/>
-    <mergeCell ref="D10:D13"/>
-    <mergeCell ref="B7:B9"/>
-    <mergeCell ref="C7:C9"/>
-    <mergeCell ref="D7:D9"/>
-    <mergeCell ref="E7:E9"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="C5:C7"/>
+    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="D5:D7"/>
+    <mergeCell ref="E5:E7"/>
+    <mergeCell ref="B15:B20"/>
+    <mergeCell ref="C15:C20"/>
+    <mergeCell ref="D15:D20"/>
+    <mergeCell ref="E15:E20"/>
+    <mergeCell ref="C11:C14"/>
+    <mergeCell ref="B11:B14"/>
+    <mergeCell ref="E11:E14"/>
+    <mergeCell ref="D11:D14"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="C8:C10"/>
+    <mergeCell ref="D8:D10"/>
+    <mergeCell ref="E8:E10"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="G18:G19 G8:G10 G5:G7" numberStoredAsText="1"/>
+    <ignoredError sqref="G19:G20 G5:G11" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Starting add AXI DMA I/F
Signed-off-by: Anderson Ignacio <anderson@aignacio.com>
</commit_message>
<xml_diff>
--- a/csr_dma.xlsx
+++ b/csr_dma.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10520"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E86F390D-0DCA-174B-9D06-3EE740FE81D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76E8CBB9-3CF0-194C-A5FF-D8975158D5D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7660" yWindow="3500" windowWidth="49080" windowHeight="24140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9160" yWindow="10860" windowWidth="49080" windowHeight="24140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="block_0" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="69">
   <si>
     <t>block name</t>
     <phoneticPr fontId="1"/>
@@ -123,12 +123,6 @@
     <t>rof</t>
   </si>
   <si>
-    <t>dma_descriptor</t>
-  </si>
-  <si>
-    <t>dest_addr</t>
-  </si>
-  <si>
     <t>src_addr</t>
   </si>
   <si>
@@ -168,9 +162,6 @@
     <t>Enable descriptor</t>
   </si>
   <si>
-    <t>dma_error</t>
-  </si>
-  <si>
     <t>error_type</t>
   </si>
   <si>
@@ -192,9 +183,6 @@
     <t>Error Trigger, asserted when error happens</t>
   </si>
   <si>
-    <t>dma_error.error_trig</t>
-  </si>
-  <si>
     <t>Error addr</t>
   </si>
   <si>
@@ -210,24 +198,12 @@
     <t>0x08</t>
   </si>
   <si>
+    <t>in the assignment = width:lsb:sequence_size:step</t>
+  </si>
+  <si>
     <t>0x20</t>
   </si>
   <si>
-    <t>32:0</t>
-  </si>
-  <si>
-    <t>1:64</t>
-  </si>
-  <si>
-    <t>32:64</t>
-  </si>
-  <si>
-    <t>32:128</t>
-  </si>
-  <si>
-    <t>1:192</t>
-  </si>
-  <si>
     <t>32</t>
   </si>
   <si>
@@ -243,14 +219,38 @@
     <t>Max burst length (ALEN) in the AXI txn</t>
   </si>
   <si>
-    <t>&gt; assignment = width:lsb:sequence_size:step</t>
+    <t>dma_error_addr</t>
+  </si>
+  <si>
+    <t>dma_error_stats</t>
+  </si>
+  <si>
+    <t>0x18</t>
+  </si>
+  <si>
+    <t>dma_desc_src_addr</t>
+  </si>
+  <si>
+    <t>dma_desc_cfg</t>
+  </si>
+  <si>
+    <t>dma_desc_dst_addr</t>
+  </si>
+  <si>
+    <t>dma_desc_num_bytes</t>
+  </si>
+  <si>
+    <t>dma_error_stats.error_trig</t>
+  </si>
+  <si>
+    <t>dst_addr</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -265,14 +265,6 @@
       <charset val="128"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -283,6 +275,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -290,12 +288,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="1"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -431,50 +423,32 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -482,7 +456,22 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -494,20 +483,32 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -792,19 +793,19 @@
   <dimension ref="B1:K70"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="210" zoomScaleNormal="210" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="13.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.1640625" style="1" customWidth="1"/>
     <col min="3" max="3" width="13" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.1640625" style="1" customWidth="1"/>
     <col min="6" max="6" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9" style="1"/>
     <col min="9" max="9" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="21.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="46.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -816,7 +817,7 @@
         <v>12</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2" spans="2:11" x14ac:dyDescent="0.2">
@@ -827,412 +828,428 @@
         <v>256</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>68</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="2:11" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B4" s="22" t="s">
+      <c r="B4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="23" t="s">
+      <c r="C4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="23" t="s">
+      <c r="D4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="24" t="s">
+      <c r="E4" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="24" t="s">
+      <c r="F4" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="24" t="s">
+      <c r="G4" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="H4" s="24" t="s">
+      <c r="H4" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="I4" s="23" t="s">
+      <c r="I4" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="J4" s="25" t="s">
+      <c r="J4" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="K4" s="26" t="s">
+      <c r="K4" s="7" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="D5" s="18"/>
+      <c r="E5" s="21"/>
+      <c r="F5" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="G5" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="H5" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="I5" s="11">
+        <v>0</v>
+      </c>
+      <c r="J5" s="9"/>
+      <c r="K5" s="11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B6" s="22"/>
+      <c r="C6" s="19"/>
+      <c r="D6" s="19"/>
+      <c r="E6" s="22"/>
+      <c r="F6" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="G6" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="H6" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="I6" s="11">
+        <v>0</v>
+      </c>
+      <c r="J6" s="9"/>
+      <c r="K6" s="11" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B7" s="23"/>
+      <c r="C7" s="20"/>
+      <c r="D7" s="20"/>
+      <c r="E7" s="23"/>
+      <c r="F7" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="G7" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="H7" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="I7" s="11">
+        <v>255</v>
+      </c>
+      <c r="J7" s="9"/>
+      <c r="K7" s="11" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="8" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B8" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="28" t="s">
+        <v>52</v>
+      </c>
+      <c r="D8" s="28"/>
+      <c r="E8" s="27"/>
+      <c r="F8" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="G8" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="H8" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="I8" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="J8" s="13"/>
+      <c r="K8" s="15" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B9" s="27"/>
+      <c r="C9" s="28"/>
+      <c r="D9" s="28"/>
+      <c r="E9" s="27"/>
+      <c r="F9" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="G9" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="H9" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="I9" s="14">
+        <v>0</v>
+      </c>
+      <c r="J9" s="13"/>
+      <c r="K9" s="15" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B10" s="27"/>
+      <c r="C10" s="28"/>
+      <c r="D10" s="28"/>
+      <c r="E10" s="27"/>
+      <c r="F10" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="G10" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="H10" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="I10" s="14">
+        <v>0</v>
+      </c>
+      <c r="J10" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="K10" s="15" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="2:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B11" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="G11" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="D5" s="4"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="G5" s="6" t="s">
+      <c r="H11" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="I11" s="10">
+        <v>0</v>
+      </c>
+      <c r="J11" s="10"/>
+      <c r="K11" s="10" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="12" spans="2:11" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B12" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="C12" s="29" t="s">
+        <v>62</v>
+      </c>
+      <c r="D12" s="29"/>
+      <c r="E12" s="18"/>
+      <c r="F12" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="G12" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="H5" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="I5" s="7">
+      <c r="H12" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="I12" s="10">
         <v>0</v>
       </c>
-      <c r="J5" s="5"/>
-      <c r="K5" s="7" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B6" s="8"/>
-      <c r="C6" s="9"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="G6" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="H6" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="I6" s="7">
-        <v>0</v>
-      </c>
-      <c r="J6" s="5"/>
-      <c r="K6" s="7" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B7" s="10"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="10"/>
-      <c r="F7" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="G7" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="H7" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="I7" s="7">
-        <v>255</v>
-      </c>
-      <c r="J7" s="5"/>
-      <c r="K7" s="7" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B8" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="C8" s="14" t="s">
-        <v>56</v>
-      </c>
-      <c r="D8" s="14"/>
-      <c r="E8" s="13"/>
-      <c r="F8" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="G8" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="H8" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="I8" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="J8" s="15"/>
-      <c r="K8" s="17" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B9" s="13"/>
-      <c r="C9" s="14"/>
-      <c r="D9" s="14"/>
-      <c r="E9" s="13"/>
-      <c r="F9" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="G9" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="H9" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="I9" s="16">
-        <v>0</v>
-      </c>
-      <c r="J9" s="15"/>
-      <c r="K9" s="17" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B10" s="13"/>
-      <c r="C10" s="14"/>
-      <c r="D10" s="14"/>
-      <c r="E10" s="13"/>
-      <c r="F10" s="15" t="s">
+      <c r="J12" s="10"/>
+      <c r="K12" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="G10" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="H10" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="I10" s="16">
-        <v>0</v>
-      </c>
-      <c r="J10" s="18" t="s">
-        <v>51</v>
-      </c>
-      <c r="K10" s="17" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B11" s="4" t="s">
+    </row>
+    <row r="13" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B13" s="29"/>
+      <c r="C13" s="29"/>
+      <c r="D13" s="29"/>
+      <c r="E13" s="19"/>
+      <c r="F13" s="12" t="s">
         <v>43</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="G11" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="H11" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="I11" s="6">
-        <v>0</v>
-      </c>
-      <c r="J11" s="6"/>
-      <c r="K11" s="6" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B12" s="9"/>
-      <c r="C12" s="9"/>
-      <c r="D12" s="9"/>
-      <c r="E12" s="9"/>
-      <c r="F12" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="G12" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="H12" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="I12" s="6">
-        <v>0</v>
-      </c>
-      <c r="J12" s="6"/>
-      <c r="K12" s="6" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B13" s="9"/>
-      <c r="C13" s="9"/>
-      <c r="D13" s="9"/>
-      <c r="E13" s="9"/>
-      <c r="F13" s="12" t="s">
-        <v>46</v>
       </c>
       <c r="G13" s="12">
         <v>1</v>
       </c>
-      <c r="H13" s="6" t="s">
+      <c r="H13" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="I13" s="6">
+      <c r="I13" s="10">
         <v>0</v>
       </c>
-      <c r="J13" s="6"/>
-      <c r="K13" s="6" t="s">
-        <v>47</v>
+      <c r="J13" s="10"/>
+      <c r="K13" s="10" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="14" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B14" s="9"/>
-      <c r="C14" s="9"/>
-      <c r="D14" s="9"/>
-      <c r="E14" s="9"/>
+      <c r="B14" s="29"/>
+      <c r="C14" s="29"/>
+      <c r="D14" s="29"/>
+      <c r="E14" s="20"/>
       <c r="F14" s="12" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="G14" s="12">
         <v>1</v>
       </c>
-      <c r="H14" s="6" t="s">
+      <c r="H14" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="I14" s="6">
+      <c r="I14" s="10">
         <v>0</v>
       </c>
-      <c r="J14" s="6"/>
-      <c r="K14" s="6" t="s">
-        <v>50</v>
+      <c r="J14" s="10"/>
+      <c r="K14" s="10" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="15" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B15" s="19" t="s">
+      <c r="B15" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="C15" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="D15" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="E15" s="17"/>
+      <c r="F15" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="C15" s="19" t="s">
-        <v>57</v>
-      </c>
-      <c r="D15" s="19" t="s">
+      <c r="G15" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="H15" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="I15" s="14">
+        <v>0</v>
+      </c>
+      <c r="J15" s="14"/>
+      <c r="K15" s="14" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B16" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="C16" s="17"/>
+      <c r="D16" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="E16" s="17"/>
+      <c r="F16" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="G16" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="H16" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="I16" s="14">
+        <v>0</v>
+      </c>
+      <c r="J16" s="14"/>
+      <c r="K16" s="14" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="17" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B17" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="C17" s="17"/>
+      <c r="D17" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="E17" s="17"/>
+      <c r="F17" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="G17" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="H17" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="I17" s="14">
+        <v>0</v>
+      </c>
+      <c r="J17" s="14"/>
+      <c r="K17" s="14" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="18" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B18" s="24" t="s">
+        <v>64</v>
+      </c>
+      <c r="C18" s="24"/>
+      <c r="D18" s="24" t="s">
+        <v>38</v>
+      </c>
+      <c r="E18" s="24"/>
+      <c r="F18" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="G18" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="H18" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="I18" s="14">
+        <v>0</v>
+      </c>
+      <c r="J18" s="14"/>
+      <c r="K18" s="14" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="19" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B19" s="25"/>
+      <c r="C19" s="25"/>
+      <c r="D19" s="25"/>
+      <c r="E19" s="25"/>
+      <c r="F19" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="G19" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="H19" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="I19" s="14">
+        <v>0</v>
+      </c>
+      <c r="J19" s="14"/>
+      <c r="K19" s="14" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="20" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B20" s="26"/>
+      <c r="C20" s="26"/>
+      <c r="D20" s="26"/>
+      <c r="E20" s="26"/>
+      <c r="F20" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="G20" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="H20" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="I20" s="14">
+        <v>0</v>
+      </c>
+      <c r="J20" s="14"/>
+      <c r="K20" s="14" t="s">
         <v>40</v>
-      </c>
-      <c r="E15" s="19"/>
-      <c r="F15" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="G15" s="15" t="s">
-        <v>58</v>
-      </c>
-      <c r="H15" s="16" t="s">
-        <v>39</v>
-      </c>
-      <c r="I15" s="16">
-        <v>0</v>
-      </c>
-      <c r="J15" s="16"/>
-      <c r="K15" s="16" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B16" s="20"/>
-      <c r="C16" s="20"/>
-      <c r="D16" s="20"/>
-      <c r="E16" s="20"/>
-      <c r="F16" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="G16" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="H16" s="16" t="s">
-        <v>39</v>
-      </c>
-      <c r="I16" s="16">
-        <v>0</v>
-      </c>
-      <c r="J16" s="16"/>
-      <c r="K16" s="16" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B17" s="20"/>
-      <c r="C17" s="20"/>
-      <c r="D17" s="20"/>
-      <c r="E17" s="20"/>
-      <c r="F17" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="G17" s="15" t="s">
-        <v>61</v>
-      </c>
-      <c r="H17" s="16" t="s">
-        <v>39</v>
-      </c>
-      <c r="I17" s="16">
-        <v>0</v>
-      </c>
-      <c r="J17" s="16"/>
-      <c r="K17" s="16" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B18" s="20"/>
-      <c r="C18" s="20"/>
-      <c r="D18" s="20"/>
-      <c r="E18" s="20"/>
-      <c r="F18" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="G18" s="15" t="s">
-        <v>62</v>
-      </c>
-      <c r="H18" s="16" t="s">
-        <v>39</v>
-      </c>
-      <c r="I18" s="16">
-        <v>0</v>
-      </c>
-      <c r="J18" s="16"/>
-      <c r="K18" s="16" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B19" s="20"/>
-      <c r="C19" s="20"/>
-      <c r="D19" s="20"/>
-      <c r="E19" s="20"/>
-      <c r="F19" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="G19" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="H19" s="16" t="s">
-        <v>39</v>
-      </c>
-      <c r="I19" s="16">
-        <v>0</v>
-      </c>
-      <c r="J19" s="16"/>
-      <c r="K19" s="16" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="20" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B20" s="21"/>
-      <c r="C20" s="21"/>
-      <c r="D20" s="21"/>
-      <c r="E20" s="21"/>
-      <c r="F20" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="G20" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="H20" s="16" t="s">
-        <v>39</v>
-      </c>
-      <c r="I20" s="16">
-        <v>0</v>
-      </c>
-      <c r="J20" s="16"/>
-      <c r="K20" s="16" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="21" spans="2:11" x14ac:dyDescent="0.2">
@@ -1371,28 +1388,28 @@
     <row r="70" customFormat="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="B18:B20"/>
+    <mergeCell ref="D18:D20"/>
+    <mergeCell ref="C18:C20"/>
+    <mergeCell ref="E18:E20"/>
     <mergeCell ref="C5:C7"/>
     <mergeCell ref="B5:B7"/>
     <mergeCell ref="D5:D7"/>
     <mergeCell ref="E5:E7"/>
-    <mergeCell ref="B15:B20"/>
-    <mergeCell ref="C15:C20"/>
-    <mergeCell ref="D15:D20"/>
-    <mergeCell ref="E15:E20"/>
-    <mergeCell ref="C11:C14"/>
-    <mergeCell ref="B11:B14"/>
-    <mergeCell ref="E11:E14"/>
-    <mergeCell ref="D11:D14"/>
     <mergeCell ref="B8:B10"/>
     <mergeCell ref="C8:C10"/>
     <mergeCell ref="D8:D10"/>
     <mergeCell ref="E8:E10"/>
+    <mergeCell ref="B12:B14"/>
+    <mergeCell ref="C12:C14"/>
+    <mergeCell ref="D12:D14"/>
+    <mergeCell ref="E12:E14"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="G19:G20 G5:G11" numberStoredAsText="1"/>
+    <ignoredError sqref="G15:G20 G5:G12" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added test for all descriptors and AXI assertions
Signed-off-by: Anderson Ignacio <anderson@aignacio.com>
</commit_message>
<xml_diff>
--- a/csr_dma.xlsx
+++ b/csr_dma.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10520"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10611"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76E8CBB9-3CF0-194C-A5FF-D8975158D5D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F91EFBFC-DF7A-DD45-9D83-98397F995DE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9160" yWindow="10860" windowWidth="49080" windowHeight="24140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="700" yWindow="4180" windowWidth="49080" windowHeight="24140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="block_0" sheetId="1" r:id="rId1"/>
+    <sheet name="csr_dma" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -186,9 +186,6 @@
     <t>Error addr</t>
   </si>
   <si>
-    <t>Error type - Operation / Configuration</t>
-  </si>
-  <si>
     <t>0x10</t>
   </si>
   <si>
@@ -244,6 +241,9 @@
   </si>
   <si>
     <t>dst_addr</t>
+  </si>
+  <si>
+    <t>Error type - 0 - Operation / 1 - Configuration</t>
   </si>
 </sst>
 </file>
@@ -423,7 +423,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -474,6 +474,18 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -490,15 +502,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -793,7 +796,7 @@
   <dimension ref="B1:K70"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="210" zoomScaleNormal="210" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -817,7 +820,7 @@
         <v>12</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="2" spans="2:11" x14ac:dyDescent="0.2">
@@ -828,7 +831,7 @@
         <v>256</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="2:11" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
@@ -865,14 +868,14 @@
       </c>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B5" s="21" t="s">
+      <c r="B5" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="18" t="s">
-        <v>51</v>
-      </c>
-      <c r="D5" s="18"/>
-      <c r="E5" s="21"/>
+      <c r="C5" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="D5" s="22"/>
+      <c r="E5" s="25"/>
       <c r="F5" s="9" t="s">
         <v>19</v>
       </c>
@@ -891,10 +894,10 @@
       </c>
     </row>
     <row r="6" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B6" s="22"/>
-      <c r="C6" s="19"/>
-      <c r="D6" s="19"/>
-      <c r="E6" s="22"/>
+      <c r="B6" s="26"/>
+      <c r="C6" s="23"/>
+      <c r="D6" s="23"/>
+      <c r="E6" s="26"/>
       <c r="F6" s="9" t="s">
         <v>20</v>
       </c>
@@ -913,15 +916,15 @@
       </c>
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B7" s="23"/>
-      <c r="C7" s="20"/>
-      <c r="D7" s="20"/>
-      <c r="E7" s="23"/>
+      <c r="B7" s="27"/>
+      <c r="C7" s="24"/>
+      <c r="D7" s="24"/>
+      <c r="E7" s="27"/>
       <c r="F7" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="G7" s="9" t="s">
         <v>57</v>
-      </c>
-      <c r="G7" s="9" t="s">
-        <v>58</v>
       </c>
       <c r="H7" s="9" t="s">
         <v>37</v>
@@ -931,18 +934,18 @@
       </c>
       <c r="J7" s="9"/>
       <c r="K7" s="11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B8" s="27" t="s">
+      <c r="B8" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="28" t="s">
-        <v>52</v>
-      </c>
-      <c r="D8" s="28"/>
-      <c r="E8" s="27"/>
+      <c r="C8" s="29" t="s">
+        <v>51</v>
+      </c>
+      <c r="D8" s="29"/>
+      <c r="E8" s="28"/>
       <c r="F8" s="13" t="s">
         <v>22</v>
       </c>
@@ -961,10 +964,10 @@
       </c>
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B9" s="27"/>
-      <c r="C9" s="28"/>
-      <c r="D9" s="28"/>
-      <c r="E9" s="27"/>
+      <c r="B9" s="28"/>
+      <c r="C9" s="29"/>
+      <c r="D9" s="29"/>
+      <c r="E9" s="28"/>
       <c r="F9" s="13" t="s">
         <v>21</v>
       </c>
@@ -983,10 +986,10 @@
       </c>
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B10" s="27"/>
-      <c r="C10" s="28"/>
-      <c r="D10" s="28"/>
-      <c r="E10" s="27"/>
+      <c r="B10" s="28"/>
+      <c r="C10" s="29"/>
+      <c r="D10" s="29"/>
+      <c r="E10" s="28"/>
       <c r="F10" s="13" t="s">
         <v>46</v>
       </c>
@@ -1000,7 +1003,7 @@
         <v>0</v>
       </c>
       <c r="J10" s="16" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="K10" s="15" t="s">
         <v>26</v>
@@ -1008,10 +1011,10 @@
     </row>
     <row r="11" spans="2:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D11" s="8"/>
       <c r="E11" s="8"/>
@@ -1019,7 +1022,7 @@
         <v>42</v>
       </c>
       <c r="G11" s="12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H11" s="10" t="s">
         <v>18</v>
@@ -1028,19 +1031,19 @@
         <v>0</v>
       </c>
       <c r="J11" s="10"/>
-      <c r="K11" s="10" t="s">
+      <c r="K11" s="18" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="12" spans="2:11" ht="14" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="29" t="s">
+      <c r="B12" s="30" t="s">
+        <v>60</v>
+      </c>
+      <c r="C12" s="30" t="s">
         <v>61</v>
       </c>
-      <c r="C12" s="29" t="s">
-        <v>62</v>
-      </c>
-      <c r="D12" s="29"/>
-      <c r="E12" s="18"/>
+      <c r="D12" s="30"/>
+      <c r="E12" s="22"/>
       <c r="F12" s="12" t="s">
         <v>41</v>
       </c>
@@ -1054,15 +1057,15 @@
         <v>0</v>
       </c>
       <c r="J12" s="10"/>
-      <c r="K12" s="10" t="s">
-        <v>49</v>
+      <c r="K12" s="18" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="13" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B13" s="29"/>
-      <c r="C13" s="29"/>
-      <c r="D13" s="29"/>
-      <c r="E13" s="19"/>
+      <c r="B13" s="30"/>
+      <c r="C13" s="30"/>
+      <c r="D13" s="30"/>
+      <c r="E13" s="23"/>
       <c r="F13" s="12" t="s">
         <v>43</v>
       </c>
@@ -1081,10 +1084,10 @@
       </c>
     </row>
     <row r="14" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B14" s="29"/>
-      <c r="C14" s="29"/>
-      <c r="D14" s="29"/>
-      <c r="E14" s="20"/>
+      <c r="B14" s="30"/>
+      <c r="C14" s="30"/>
+      <c r="D14" s="30"/>
+      <c r="E14" s="24"/>
       <c r="F14" s="12" t="s">
         <v>45</v>
       </c>
@@ -1104,10 +1107,10 @@
     </row>
     <row r="15" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B15" s="17" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C15" s="17" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D15" s="17" t="s">
         <v>38</v>
@@ -1117,7 +1120,7 @@
         <v>28</v>
       </c>
       <c r="G15" s="13" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H15" s="14" t="s">
         <v>37</v>
@@ -1132,7 +1135,7 @@
     </row>
     <row r="16" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B16" s="17" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C16" s="17"/>
       <c r="D16" s="17" t="s">
@@ -1140,10 +1143,10 @@
       </c>
       <c r="E16" s="17"/>
       <c r="F16" s="13" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G16" s="13" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H16" s="14" t="s">
         <v>37</v>
@@ -1158,7 +1161,7 @@
     </row>
     <row r="17" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B17" s="17" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C17" s="17"/>
       <c r="D17" s="17" t="s">
@@ -1169,7 +1172,7 @@
         <v>29</v>
       </c>
       <c r="G17" s="13" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H17" s="14" t="s">
         <v>37</v>
@@ -1183,14 +1186,14 @@
       </c>
     </row>
     <row r="18" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B18" s="24" t="s">
-        <v>64</v>
-      </c>
-      <c r="C18" s="24"/>
-      <c r="D18" s="24" t="s">
+      <c r="B18" s="19" t="s">
+        <v>63</v>
+      </c>
+      <c r="C18" s="19"/>
+      <c r="D18" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="E18" s="24"/>
+      <c r="E18" s="19"/>
       <c r="F18" s="13" t="s">
         <v>32</v>
       </c>
@@ -1209,10 +1212,10 @@
       </c>
     </row>
     <row r="19" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B19" s="25"/>
-      <c r="C19" s="25"/>
-      <c r="D19" s="25"/>
-      <c r="E19" s="25"/>
+      <c r="B19" s="20"/>
+      <c r="C19" s="20"/>
+      <c r="D19" s="20"/>
+      <c r="E19" s="20"/>
       <c r="F19" s="13" t="s">
         <v>31</v>
       </c>
@@ -1231,10 +1234,10 @@
       </c>
     </row>
     <row r="20" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B20" s="26"/>
-      <c r="C20" s="26"/>
-      <c r="D20" s="26"/>
-      <c r="E20" s="26"/>
+      <c r="B20" s="21"/>
+      <c r="C20" s="21"/>
+      <c r="D20" s="21"/>
+      <c r="E20" s="21"/>
       <c r="F20" s="13" t="s">
         <v>39</v>
       </c>

</xml_diff>

<commit_message>
Added max burst test
Signed-off-by: Anderson Ignacio <anderson@aignacio.com>
</commit_message>
<xml_diff>
--- a/csr_dma.xlsx
+++ b/csr_dma.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10611"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F91EFBFC-DF7A-DD45-9D83-98397F995DE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{018D9AE8-A0E5-E54C-A9EB-CED9B8212E14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="700" yWindow="4180" windowWidth="49080" windowHeight="24140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -796,7 +796,7 @@
   <dimension ref="B1:K70"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="210" zoomScaleNormal="210" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1009,7 +1009,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="2:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B11" s="8" t="s">
         <v>59</v>
       </c>

</xml_diff>

<commit_message>
Added parameters to shrink the design size
Signed-off-by: Anderson Ignacio <anderson@aignacio.com>
</commit_message>
<xml_diff>
--- a/csr_dma.xlsx
+++ b/csr_dma.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11011"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{018D9AE8-A0E5-E54C-A9EB-CED9B8212E14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{DAF35122-2101-7E4D-893F-37498E040341}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="700" yWindow="4180" windowWidth="49080" windowHeight="24140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="700" yWindow="4180" windowWidth="71920" windowHeight="26240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="csr_dma" sheetId="1" r:id="rId1"/>
@@ -153,9 +153,6 @@
     <t>rw</t>
   </si>
   <si>
-    <t>[5]</t>
-  </si>
-  <si>
     <t>enable</t>
   </si>
   <si>
@@ -244,6 +241,9 @@
   </si>
   <si>
     <t>Error type - 0 - Operation / 1 - Configuration</t>
+  </si>
+  <si>
+    <t>[2]</t>
   </si>
 </sst>
 </file>
@@ -423,7 +423,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -472,9 +472,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -796,7 +793,7 @@
   <dimension ref="B1:K70"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="210" zoomScaleNormal="210" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="D12" sqref="D12:D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -820,7 +817,7 @@
         <v>12</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="2" spans="2:11" x14ac:dyDescent="0.2">
@@ -831,7 +828,7 @@
         <v>256</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="2:11" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
@@ -868,14 +865,14 @@
       </c>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B5" s="25" t="s">
+      <c r="B5" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="22" t="s">
-        <v>50</v>
-      </c>
-      <c r="D5" s="22"/>
-      <c r="E5" s="25"/>
+      <c r="C5" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="D5" s="21"/>
+      <c r="E5" s="24"/>
       <c r="F5" s="9" t="s">
         <v>19</v>
       </c>
@@ -894,10 +891,10 @@
       </c>
     </row>
     <row r="6" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B6" s="26"/>
-      <c r="C6" s="23"/>
-      <c r="D6" s="23"/>
-      <c r="E6" s="26"/>
+      <c r="B6" s="25"/>
+      <c r="C6" s="22"/>
+      <c r="D6" s="22"/>
+      <c r="E6" s="25"/>
       <c r="F6" s="9" t="s">
         <v>20</v>
       </c>
@@ -916,15 +913,15 @@
       </c>
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B7" s="27"/>
-      <c r="C7" s="24"/>
-      <c r="D7" s="24"/>
-      <c r="E7" s="27"/>
+      <c r="B7" s="26"/>
+      <c r="C7" s="23"/>
+      <c r="D7" s="23"/>
+      <c r="E7" s="26"/>
       <c r="F7" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="G7" s="9" t="s">
         <v>56</v>
-      </c>
-      <c r="G7" s="9" t="s">
-        <v>57</v>
       </c>
       <c r="H7" s="9" t="s">
         <v>37</v>
@@ -934,18 +931,18 @@
       </c>
       <c r="J7" s="9"/>
       <c r="K7" s="11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B8" s="28" t="s">
+      <c r="B8" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="29" t="s">
-        <v>51</v>
-      </c>
-      <c r="D8" s="29"/>
-      <c r="E8" s="28"/>
+      <c r="C8" s="28" t="s">
+        <v>50</v>
+      </c>
+      <c r="D8" s="28"/>
+      <c r="E8" s="27"/>
       <c r="F8" s="13" t="s">
         <v>22</v>
       </c>
@@ -964,10 +961,10 @@
       </c>
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B9" s="28"/>
-      <c r="C9" s="29"/>
-      <c r="D9" s="29"/>
-      <c r="E9" s="28"/>
+      <c r="B9" s="27"/>
+      <c r="C9" s="28"/>
+      <c r="D9" s="28"/>
+      <c r="E9" s="27"/>
       <c r="F9" s="13" t="s">
         <v>21</v>
       </c>
@@ -986,12 +983,12 @@
       </c>
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B10" s="28"/>
-      <c r="C10" s="29"/>
-      <c r="D10" s="29"/>
-      <c r="E10" s="28"/>
+      <c r="B10" s="27"/>
+      <c r="C10" s="28"/>
+      <c r="D10" s="28"/>
+      <c r="E10" s="27"/>
       <c r="F10" s="13" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G10" s="14" t="s">
         <v>11</v>
@@ -1003,7 +1000,7 @@
         <v>0</v>
       </c>
       <c r="J10" s="16" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="K10" s="15" t="s">
         <v>26</v>
@@ -1011,18 +1008,18 @@
     </row>
     <row r="11" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B11" s="8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D11" s="8"/>
       <c r="E11" s="8"/>
       <c r="F11" s="12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G11" s="12" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H11" s="10" t="s">
         <v>18</v>
@@ -1031,21 +1028,21 @@
         <v>0</v>
       </c>
       <c r="J11" s="10"/>
-      <c r="K11" s="18" t="s">
-        <v>48</v>
+      <c r="K11" s="10" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="12" spans="2:11" ht="14" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="30" t="s">
+      <c r="B12" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="C12" s="29" t="s">
         <v>60</v>
       </c>
-      <c r="C12" s="30" t="s">
-        <v>61</v>
-      </c>
-      <c r="D12" s="30"/>
-      <c r="E12" s="22"/>
+      <c r="D12" s="29"/>
+      <c r="E12" s="21"/>
       <c r="F12" s="12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G12" s="12" t="s">
         <v>11</v>
@@ -1057,17 +1054,17 @@
         <v>0</v>
       </c>
       <c r="J12" s="10"/>
-      <c r="K12" s="18" t="s">
-        <v>68</v>
+      <c r="K12" s="10" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="13" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B13" s="30"/>
-      <c r="C13" s="30"/>
-      <c r="D13" s="30"/>
-      <c r="E13" s="23"/>
+      <c r="B13" s="29"/>
+      <c r="C13" s="29"/>
+      <c r="D13" s="29"/>
+      <c r="E13" s="22"/>
       <c r="F13" s="12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G13" s="12">
         <v>1</v>
@@ -1080,16 +1077,16 @@
       </c>
       <c r="J13" s="10"/>
       <c r="K13" s="10" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="14" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B14" s="29"/>
+      <c r="C14" s="29"/>
+      <c r="D14" s="29"/>
+      <c r="E14" s="23"/>
+      <c r="F14" s="12" t="s">
         <v>44</v>
-      </c>
-    </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B14" s="30"/>
-      <c r="C14" s="30"/>
-      <c r="D14" s="30"/>
-      <c r="E14" s="24"/>
-      <c r="F14" s="12" t="s">
-        <v>45</v>
       </c>
       <c r="G14" s="12">
         <v>1</v>
@@ -1102,25 +1099,25 @@
       </c>
       <c r="J14" s="10"/>
       <c r="K14" s="10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="15" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B15" s="17" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C15" s="17" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D15" s="17" t="s">
-        <v>38</v>
+        <v>68</v>
       </c>
       <c r="E15" s="17"/>
       <c r="F15" s="13" t="s">
         <v>28</v>
       </c>
       <c r="G15" s="13" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H15" s="14" t="s">
         <v>37</v>
@@ -1135,18 +1132,18 @@
     </row>
     <row r="16" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B16" s="17" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C16" s="17"/>
       <c r="D16" s="17" t="s">
-        <v>38</v>
+        <v>68</v>
       </c>
       <c r="E16" s="17"/>
       <c r="F16" s="13" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G16" s="13" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H16" s="14" t="s">
         <v>37</v>
@@ -1161,18 +1158,18 @@
     </row>
     <row r="17" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B17" s="17" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C17" s="17"/>
       <c r="D17" s="17" t="s">
-        <v>38</v>
+        <v>68</v>
       </c>
       <c r="E17" s="17"/>
       <c r="F17" s="13" t="s">
         <v>29</v>
       </c>
       <c r="G17" s="13" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H17" s="14" t="s">
         <v>37</v>
@@ -1186,14 +1183,14 @@
       </c>
     </row>
     <row r="18" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B18" s="19" t="s">
-        <v>63</v>
-      </c>
-      <c r="C18" s="19"/>
-      <c r="D18" s="19" t="s">
-        <v>38</v>
-      </c>
-      <c r="E18" s="19"/>
+      <c r="B18" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="C18" s="18"/>
+      <c r="D18" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="E18" s="18"/>
       <c r="F18" s="13" t="s">
         <v>32</v>
       </c>
@@ -1212,10 +1209,10 @@
       </c>
     </row>
     <row r="19" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B19" s="20"/>
-      <c r="C19" s="20"/>
-      <c r="D19" s="20"/>
-      <c r="E19" s="20"/>
+      <c r="B19" s="19"/>
+      <c r="C19" s="19"/>
+      <c r="D19" s="19"/>
+      <c r="E19" s="19"/>
       <c r="F19" s="13" t="s">
         <v>31</v>
       </c>
@@ -1234,12 +1231,12 @@
       </c>
     </row>
     <row r="20" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B20" s="21"/>
-      <c r="C20" s="21"/>
-      <c r="D20" s="21"/>
-      <c r="E20" s="21"/>
+      <c r="B20" s="20"/>
+      <c r="C20" s="20"/>
+      <c r="D20" s="20"/>
+      <c r="E20" s="20"/>
       <c r="F20" s="13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G20" s="13" t="s">
         <v>11</v>
@@ -1252,7 +1249,7 @@
       </c>
       <c r="J20" s="14"/>
       <c r="K20" s="14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="21" spans="2:11" x14ac:dyDescent="0.2">

</xml_diff>